<commit_message>
MAJ fichier  specifications et dictionnaire des données cibles
</commit_message>
<xml_diff>
--- a/documentation/donnees_cibles/dictionnaire_données_fichiers_cibles.xlsx
+++ b/documentation/donnees_cibles/dictionnaire_données_fichiers_cibles.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferdinand.mabille\Documents\Git\Demographie_professionnels_sante\documentation\donnees_cibles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferdinand.mabille\Documents\Git\Demographie_professionnels_sante_old\documentation\donnees_cibles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Activités.csv" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="211">
   <si>
     <t>VARIABLE</t>
   </si>
@@ -34,12 +34,6 @@
   </si>
   <si>
     <t>CONTRAINTES</t>
-  </si>
-  <si>
-    <t>INTEGER</t>
-  </si>
-  <si>
-    <t>INTEGER / TEXT</t>
   </si>
   <si>
     <t>TEXT</t>
@@ -276,15 +270,6 @@
     <t>Extraction_RPPS_Profil1_ReferAe.csv ;</t>
   </si>
   <si>
-    <t>Extraction_RPPS_Profil1_ReferAe.csv ; ? Extraction_RPPS_Profil1_ExercPro.csv (Code AE 1e inscription) ? ;</t>
-  </si>
-  <si>
-    <t>Extraction_RPPS_Profil1_ReferAe.csv ;  ? Extraction_RPPS_Profil1_ExercPro.csv (Libellé AE 1e inscription) ? ;</t>
-  </si>
-  <si>
-    <t>Extraction_RPPS_Profil1_ReferAe.csv ; ? Extraction_RPPS_Profil1_ExercPro.csv (Date début 1e inscription) ? ;</t>
-  </si>
-  <si>
     <t>DEPARTEMENT_COORD_CORRESPONDANCE</t>
   </si>
   <si>
@@ -672,27 +657,26 @@
     <t>Extraction_RPPS_Profil1_DiplObt.csv</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Extraction_RPPS_Profil1_Personne.csv ;</t>
   </si>
   <si>
     <t xml:space="preserve">Extraction_RPPS_Profil1_Personne.csv ; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extraction_RPPS_Profil1_ReferAe.csv ; </t>
+  </si>
+  <si>
+    <t>departement2020.csv</t>
+  </si>
+  <si>
+    <t>region2020.csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -724,7 +708,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -750,14 +733,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -767,10 +750,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1054,17 +1038,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A45" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="42.85546875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1075,781 +1059,781 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="C2" s="2"/>
       <c r="E2" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="C3" s="2"/>
       <c r="E3" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="C4" s="2"/>
       <c r="E4" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="C5" s="2"/>
       <c r="E5" s="7" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" s="3"/>
       <c r="E6" s="7" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="3"/>
       <c r="E7" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C8" s="3"/>
       <c r="E8" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="C9" s="3"/>
       <c r="E9" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C10" s="3"/>
       <c r="E10" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>15</v>
+      <c r="A11" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C11" s="3"/>
       <c r="E11" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C12" s="3"/>
       <c r="E12" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C13" s="3"/>
       <c r="E13" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C14" s="3"/>
       <c r="E14" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="3"/>
       <c r="E15" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C16" s="3"/>
       <c r="E16" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C17" s="3"/>
       <c r="E17" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C18" s="3"/>
       <c r="E18" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C19" s="3"/>
       <c r="E19" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C20" s="3"/>
       <c r="E20" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C21" s="3"/>
       <c r="E21" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="3"/>
       <c r="E22" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C23" s="3"/>
       <c r="E23" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C24" s="3"/>
       <c r="E24" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C25" s="3"/>
       <c r="E25" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C26" s="3"/>
       <c r="E26" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C27" s="3"/>
       <c r="E27" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C28" s="3"/>
       <c r="E28" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C29" s="3"/>
       <c r="E29" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C30" s="3"/>
       <c r="E30" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C31" s="3"/>
       <c r="E31" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C32" s="3"/>
       <c r="E32" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C33" s="3"/>
       <c r="E33" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C34" s="3"/>
       <c r="E34" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C35" s="3"/>
       <c r="E35" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C36" s="3"/>
       <c r="E36" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C37" s="3"/>
       <c r="E37" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C38" s="3"/>
       <c r="E38" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C39" s="3"/>
       <c r="E39" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C40" s="3"/>
       <c r="E40" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C41" s="3"/>
       <c r="E41" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C42" s="3"/>
       <c r="E42" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C43" s="3"/>
       <c r="E43" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C44" s="3"/>
       <c r="E44" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C45" s="3"/>
       <c r="E45" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C46" s="3"/>
       <c r="E46" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C47" s="3"/>
       <c r="E47" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C48" s="3"/>
       <c r="E48" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C49" s="3"/>
       <c r="E49" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C50" s="3"/>
       <c r="E50" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C51" s="3"/>
       <c r="E51" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C52" s="3"/>
       <c r="E52" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C53" s="3"/>
       <c r="E53" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C54" s="3"/>
       <c r="E54" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C55" s="3"/>
       <c r="E55" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C56" s="3"/>
       <c r="E56" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C57" s="3"/>
       <c r="E57" s="5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C58" s="3"/>
       <c r="E58" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C59" s="3"/>
       <c r="E59" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C60" s="3"/>
       <c r="E60" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C61" s="3"/>
       <c r="E61" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C62" s="3"/>
       <c r="E62" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C63" s="3"/>
       <c r="E63" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C64" s="3"/>
       <c r="E64" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C65" s="3"/>
       <c r="E65" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1862,14 +1846,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
       <selection sqref="A1:E122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.140625" style="5" bestFit="1" customWidth="1"/>
@@ -1879,1348 +1863,1348 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>211</v>
+        <v>77</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>211</v>
+        <v>78</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="E4" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>79</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>93</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>4</v>
+        <v>88</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>98</v>
-      </c>
-      <c r="B21" t="s">
-        <v>5</v>
+        <v>93</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>99</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>4</v>
+        <v>94</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>100</v>
-      </c>
-      <c r="B23" t="s">
-        <v>5</v>
+        <v>95</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>101</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>4</v>
+        <v>96</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>102</v>
-      </c>
-      <c r="B25" t="s">
-        <v>5</v>
+        <v>97</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>103</v>
-      </c>
-      <c r="B26" t="s">
-        <v>5</v>
+        <v>98</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>104</v>
-      </c>
-      <c r="B27" t="s">
-        <v>5</v>
+        <v>99</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>105</v>
-      </c>
-      <c r="B28" t="s">
-        <v>5</v>
+        <v>100</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>106</v>
-      </c>
-      <c r="B29" t="s">
-        <v>5</v>
+        <v>101</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>107</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>4</v>
+        <v>102</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>108</v>
-      </c>
-      <c r="B31" t="s">
-        <v>5</v>
+        <v>103</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>109</v>
-      </c>
-      <c r="B32" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>110</v>
-      </c>
-      <c r="B33" t="s">
-        <v>5</v>
+        <v>105</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>111</v>
-      </c>
-      <c r="B34" t="s">
-        <v>5</v>
+        <v>106</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>112</v>
-      </c>
-      <c r="B35" t="s">
-        <v>5</v>
+        <v>107</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>113</v>
-      </c>
-      <c r="B36" t="s">
-        <v>5</v>
+        <v>108</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>114</v>
-      </c>
-      <c r="B37" t="s">
-        <v>5</v>
+        <v>109</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>115</v>
-      </c>
-      <c r="B38" t="s">
+        <v>110</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>116</v>
-      </c>
-      <c r="B39" t="s">
-        <v>5</v>
+        <v>111</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>117</v>
-      </c>
-      <c r="B40" t="s">
-        <v>5</v>
+        <v>112</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>118</v>
-      </c>
-      <c r="B41" t="s">
-        <v>5</v>
+        <v>113</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>119</v>
-      </c>
-      <c r="B42" t="s">
-        <v>5</v>
+        <v>114</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>120</v>
-      </c>
-      <c r="B43" t="s">
-        <v>5</v>
+        <v>115</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>121</v>
-      </c>
-      <c r="B44" t="s">
-        <v>5</v>
+        <v>116</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>122</v>
-      </c>
-      <c r="B45" t="s">
+        <v>117</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>123</v>
-      </c>
-      <c r="B46" t="s">
+        <v>118</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>124</v>
-      </c>
-      <c r="B47" t="s">
-        <v>5</v>
+        <v>119</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>125</v>
-      </c>
-      <c r="B48" t="s">
+        <v>120</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>126</v>
-      </c>
-      <c r="B49" t="s">
-        <v>5</v>
+        <v>121</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>127</v>
-      </c>
-      <c r="B50" t="s">
+        <v>122</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>128</v>
-      </c>
-      <c r="B51" t="s">
+        <v>123</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>129</v>
-      </c>
-      <c r="B52" t="s">
+        <v>124</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>130</v>
-      </c>
-      <c r="B53" t="s">
-        <v>5</v>
+        <v>125</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>131</v>
-      </c>
-      <c r="B54" t="s">
-        <v>5</v>
+        <v>126</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>132</v>
-      </c>
-      <c r="B55" t="s">
-        <v>5</v>
+        <v>127</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>133</v>
-      </c>
-      <c r="B56" t="s">
+        <v>128</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>134</v>
-      </c>
-      <c r="B57" t="s">
+        <v>129</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>135</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>4</v>
+        <v>130</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>136</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>4</v>
+        <v>131</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>137</v>
-      </c>
-      <c r="B60" t="s">
+        <v>132</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>138</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>4</v>
+        <v>133</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>139</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>4</v>
+        <v>134</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>143</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>4</v>
+        <v>138</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>158</v>
-      </c>
-      <c r="B81" t="s">
+        <v>153</v>
+      </c>
+      <c r="B81" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>159</v>
-      </c>
-      <c r="B82" t="s">
+        <v>154</v>
+      </c>
+      <c r="B82" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E82" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E83" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>161</v>
-      </c>
-      <c r="B84" t="s">
+        <v>156</v>
+      </c>
+      <c r="B84" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E84" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E85" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>163</v>
-      </c>
-      <c r="B86" t="s">
+        <v>158</v>
+      </c>
+      <c r="B86" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E86" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>164</v>
-      </c>
-      <c r="B87" t="s">
+        <v>159</v>
+      </c>
+      <c r="B87" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>165</v>
-      </c>
-      <c r="B88" t="s">
+        <v>160</v>
+      </c>
+      <c r="B88" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E88" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E89" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E90" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E91" s="7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E92" s="7" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E96" s="7" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E98" s="7" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E99" s="7" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E105" s="7" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E108" s="7" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E110" s="7" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>188</v>
-      </c>
-      <c r="B111" t="s">
-        <v>5</v>
+        <v>183</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E111" s="7" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>189</v>
-      </c>
-      <c r="B112" t="s">
-        <v>5</v>
+        <v>184</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E112" s="7" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>190</v>
-      </c>
-      <c r="B113" t="s">
-        <v>5</v>
+        <v>185</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E113" s="7" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>191</v>
-      </c>
-      <c r="B114" t="s">
-        <v>5</v>
+        <v>186</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E114" s="7" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>192</v>
-      </c>
-      <c r="B115" t="s">
-        <v>5</v>
+        <v>187</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E115" s="7" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>193</v>
-      </c>
-      <c r="B116" t="s">
-        <v>5</v>
+        <v>188</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E116" s="7" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>194</v>
-      </c>
-      <c r="B117" t="s">
-        <v>5</v>
+        <v>189</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E117" s="7" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>195</v>
-      </c>
-      <c r="B118" t="s">
-        <v>5</v>
+        <v>190</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E118" s="7" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>196</v>
-      </c>
-      <c r="B119" t="s">
-        <v>5</v>
+        <v>191</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E119" s="7" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>197</v>
-      </c>
-      <c r="B120" t="s">
-        <v>5</v>
+        <v>192</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E120" s="7" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>198</v>
-      </c>
-      <c r="B121" t="s">
-        <v>5</v>
+        <v>193</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E121" s="7" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>199</v>
-      </c>
-      <c r="B122" t="s">
-        <v>5</v>
+        <v>194</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E122" s="7" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>